<commit_message>
double purification and small bug in megastructure composition
</commit_message>
<xml_diff>
--- a/core_plates/sw_src004_polyAgridiron.xlsx
+++ b/core_plates/sw_src004_polyAgridiron.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stellawang/Dropbox (HMS)/sequences/platelayouts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stellawang/Documents/gitrepos/Crisscross-Design/core_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39E2CD7-D795-E945-BAB6-701F9982140F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F45D43-1B17-1448-B2E7-AFC2A426EFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26060" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-55600" yWindow="-7220" windowWidth="26060" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Names" sheetId="1" r:id="rId1"/>
     <sheet name="Sequences" sheetId="2" r:id="rId2"/>
+    <sheet name="Descriptions" sheetId="4" r:id="rId3"/>
+    <sheet name="Extra Transfers" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="139">
   <si>
     <t>sw_src004</t>
   </si>
@@ -326,9 +328,6 @@
     <t>from P3299_SW</t>
   </si>
   <si>
-    <t>from P????_SW</t>
-  </si>
-  <si>
     <t>GCCAGCAAAATGTTTATGTAGATGAAGGTATACACAACTACCAAAAAAAAAAAAAAAAAAAAAAAAA</t>
   </si>
   <si>
@@ -423,30 +422,69 @@
   </si>
   <si>
     <t>AAGAGAAGGATGCCCACGCATAACCGATATAT TTCCTCTTCT CACAACTACC AAAAAAAAAAAAAAAAAAAAAAAAA</t>
+  </si>
+  <si>
+    <t>CTTGAAAACATAGATGATGAAACAAAACAAA TT CTCCTCAATC ACTATTCCTATTATAACTATACTT</t>
+  </si>
+  <si>
+    <t>CTTGAAAACATAGATGATGAAACAAAACAAA TT ACTATTCCTATTATAACTATACTT CTCCTCAATC</t>
+  </si>
+  <si>
+    <t>Double purification handles</t>
+  </si>
+  <si>
+    <t>SSW041DoublePurification5primetoehold_h2_pos32</t>
+  </si>
+  <si>
+    <t>SSW042DoublePurification3primetoehold_h2_pos32</t>
+  </si>
+  <si>
+    <t>NAX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,8 +509,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -624,18 +668,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -645,17 +703,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -669,9 +724,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E95EC0C9-D135-5D4F-A941-F5710E23E724}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1831,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1926,127 +1992,127 @@
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="O2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="P2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="R2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="S2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="T2" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="U2" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="20" t="s">
+      <c r="V2" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="W2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="20" t="s">
+      <c r="X2" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="20" t="s">
+      <c r="Y2" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="24" t="s">
+      <c r="Z2" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="23" t="s">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23" t="s">
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="23" t="s">
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="23" t="s">
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="23" t="s">
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="X3" s="22"/>
-      <c r="Y3" s="22"/>
-      <c r="Z3" s="23" t="s">
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="22" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2054,31 +2120,35 @@
       <c r="A4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21"/>
-      <c r="Y4" s="21"/>
-      <c r="Z4" s="25"/>
+      <c r="B4" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="24"/>
     </row>
     <row r="5" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -2471,187 +2541,763 @@
       <c r="Z17" s="11"/>
     </row>
     <row r="18" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="2" t="s">
+      <c r="Z18" s="11"/>
+    </row>
+    <row r="19" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z19" s="11"/>
+    </row>
+    <row r="20" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z20" s="11"/>
+    </row>
+    <row r="21" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z21" s="11"/>
+    </row>
+    <row r="22" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z22" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Z22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
+    <col min="2" max="25" width="6.1640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="27.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="10.83203125" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P18" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q18" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R18" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S18" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T18" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V18" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W18" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X18" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y18" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z18" s="11"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" spans="1:26" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="30.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+    </row>
+    <row r="6" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+      <c r="X11" s="11"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
+      <c r="X12" s="11"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+    </row>
+    <row r="17" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="11"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="15"/>
     </row>
     <row r="19" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="N19" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="O19" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="P19" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q19" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="R19" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="S19" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="T19" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="U19" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="V19" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="W19" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="X19" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y19" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z19" s="11"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="16"/>
+      <c r="Z19" s="15"/>
     </row>
     <row r="20" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
       <c r="Z20" s="11"/>
     </row>
     <row r="21" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2712,242 +3358,642 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup scale="60" orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:Z22"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043AC3E2-AC2C-7847-82AD-69DD83BABFAC}">
+  <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="107" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
-    <col min="2" max="25" width="6.1640625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="27.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="10.83203125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4"/>
-    </row>
-    <row r="2" spans="1:26" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="30.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="P2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="S2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="T2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="V2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="X2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y2" s="30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" s="31"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="32"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="32"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA9AD6F-7108-C54F-83FD-B6F168ADBE58}">
+  <dimension ref="A1:Y5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -2971,13 +4017,10 @@
       <c r="W4" s="11"/>
       <c r="X4" s="11"/>
       <c r="Y4" s="11"/>
-      <c r="Z4" s="12"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="2"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -3001,617 +4044,8 @@
       <c r="W5" s="11"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-    </row>
-    <row r="13" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-    </row>
-    <row r="17" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="11"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="N18" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="O18" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="P18" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q18" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="R18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="S18" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="T18" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="U18" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="V18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="W18" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="X18" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y18" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z18" s="16"/>
-    </row>
-    <row r="19" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="M19" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="N19" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="O19" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="P19" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q19" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="R19" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="S19" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="T19" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="U19" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="V19" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="W19" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="X19" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y19" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z19" s="16"/>
-    </row>
-    <row r="20" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="11"/>
-    </row>
-    <row r="21" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
-      <c r="Z21" s="11"/>
-    </row>
-    <row r="22" spans="1:26" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" orientation="landscape"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>